<commit_message>
order cols in helper_func_module/plot_func.py plots.page0()
</commit_message>
<xml_diff>
--- a/input_output/input_dir/DFII10.xlsx
+++ b/input_output/input_dir/DFII10.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Mac\Home\Python_Projects\sp500_earn_price\input_output\input_dir\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBAFF32F-BA53-4063-8814-007E24067B85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1A6FFB7-CC98-4492-A815-1D3CD9D441DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1553" yWindow="0" windowWidth="21487" windowHeight="13680" xr2:uid="{663B75C4-4EF0-43BA-B2A2-705907C78B86}"/>
+    <workbookView xWindow="1470" yWindow="720" windowWidth="21487" windowHeight="13680" xr2:uid="{663B75C4-4EF0-43BA-B2A2-705907C78B86}"/>
   </bookViews>
   <sheets>
     <sheet name="FRED Graph" sheetId="1" r:id="rId1"/>
@@ -423,10 +423,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23184F55-AF2F-421E-BC51-13A1C6FC6898}">
-  <dimension ref="A1:B103"/>
+  <dimension ref="A1:B104"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A88" workbookViewId="0">
-      <selection activeCell="B104" sqref="B104"/>
+      <selection activeCell="B105" sqref="B105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.6640625" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
@@ -1218,6 +1218,14 @@
         <v>2.14</v>
       </c>
     </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A104" s="1">
+        <v>45694</v>
+      </c>
+      <c r="B104" s="2">
+        <v>2.0299999999999998</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Fix bugs & Add branch initial setup vs update
</commit_message>
<xml_diff>
--- a/input_output/input_dir/DFII10.xlsx
+++ b/input_output/input_dir/DFII10.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Mac\Home\Python_Projects\sp500_earn_price\input_output\input_dir\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1A6FFB7-CC98-4492-A815-1D3CD9D441DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B17CE691-8F3A-41A6-8FD5-D07F2E56AAF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1470" yWindow="720" windowWidth="21487" windowHeight="13680" xr2:uid="{663B75C4-4EF0-43BA-B2A2-705907C78B86}"/>
+    <workbookView xWindow="1553" yWindow="720" windowWidth="21487" windowHeight="13680" xr2:uid="{663B75C4-4EF0-43BA-B2A2-705907C78B86}"/>
   </bookViews>
   <sheets>
     <sheet name="FRED Graph" sheetId="1" r:id="rId1"/>
@@ -423,10 +423,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23184F55-AF2F-421E-BC51-13A1C6FC6898}">
-  <dimension ref="A1:B104"/>
+  <dimension ref="A1:B105"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A88" workbookViewId="0">
-      <selection activeCell="B105" sqref="B105"/>
+      <selection activeCell="A106" sqref="A106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.6640625" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
@@ -1226,6 +1226,14 @@
         <v>2.0299999999999998</v>
       </c>
     </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A105" s="1">
+        <v>45699</v>
+      </c>
+      <c r="B105" s="2">
+        <v>2.08</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
update .gitignore and removed cached files
</commit_message>
<xml_diff>
--- a/input_output/input_dir/DFII10.xlsx
+++ b/input_output/input_dir/DFII10.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Mac\Home\Python_Projects\sp500_earn_price\input_output\input_dir\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B17CE691-8F3A-41A6-8FD5-D07F2E56AAF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEA6C9F4-8A4E-4987-82EB-C7C06412D65D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1553" yWindow="720" windowWidth="21487" windowHeight="13680" xr2:uid="{663B75C4-4EF0-43BA-B2A2-705907C78B86}"/>
+    <workbookView xWindow="75" yWindow="15" windowWidth="22702" windowHeight="13590" xr2:uid="{663B75C4-4EF0-43BA-B2A2-705907C78B86}"/>
   </bookViews>
   <sheets>
     <sheet name="FRED Graph" sheetId="1" r:id="rId1"/>
@@ -423,10 +423,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23184F55-AF2F-421E-BC51-13A1C6FC6898}">
-  <dimension ref="A1:B105"/>
+  <dimension ref="A1:B107"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A88" workbookViewId="0">
-      <selection activeCell="A106" sqref="A106"/>
+    <sheetView tabSelected="1" topLeftCell="A87" workbookViewId="0">
+      <selection activeCell="A108" sqref="A108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.6640625" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
@@ -1234,6 +1234,22 @@
         <v>2.08</v>
       </c>
     </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A106" s="1">
+        <v>45706</v>
+      </c>
+      <c r="B106" s="2">
+        <v>2.1</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A107" s="1">
+        <v>45716</v>
+      </c>
+      <c r="B107" s="2">
+        <v>1.86</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Fix various problems in update.py and display.py
</commit_message>
<xml_diff>
--- a/input_output/input_dir/DFII10.xlsx
+++ b/input_output/input_dir/DFII10.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Mac\Home\Python_Projects\sp500_earn_price\input_output\input_dir\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEA6C9F4-8A4E-4987-82EB-C7C06412D65D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76A34430-E291-4388-BE89-C25E9C52C5C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="75" yWindow="15" windowWidth="22702" windowHeight="13590" xr2:uid="{663B75C4-4EF0-43BA-B2A2-705907C78B86}"/>
+    <workbookView xWindow="338" yWindow="338" windowWidth="21217" windowHeight="12592" xr2:uid="{663B75C4-4EF0-43BA-B2A2-705907C78B86}"/>
   </bookViews>
   <sheets>
     <sheet name="FRED Graph" sheetId="1" r:id="rId1"/>
@@ -423,10 +423,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23184F55-AF2F-421E-BC51-13A1C6FC6898}">
-  <dimension ref="A1:B107"/>
+  <dimension ref="A1:B108"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A87" workbookViewId="0">
-      <selection activeCell="A108" sqref="A108"/>
+      <selection activeCell="B109" sqref="B109"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.6640625" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
@@ -1244,10 +1244,18 @@
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A107" s="1">
-        <v>45716</v>
+        <v>45747</v>
       </c>
       <c r="B107" s="2">
-        <v>1.86</v>
+        <v>1.85</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A108" s="1">
+        <v>45777</v>
+      </c>
+      <c r="B108" s="2">
+        <v>1.94</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Use frozen dataclass to fix constants
</commit_message>
<xml_diff>
--- a/input_output/input_dir/DFII10.xlsx
+++ b/input_output/input_dir/DFII10.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Mac\Home\Python_Projects\sp500_earn_price\input_output\input_dir\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76A34430-E291-4388-BE89-C25E9C52C5C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54B2388B-4F60-43A2-BD65-EDE3CCC837B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="338" yWindow="338" windowWidth="21217" windowHeight="12592" xr2:uid="{663B75C4-4EF0-43BA-B2A2-705907C78B86}"/>
+    <workbookView xWindow="675" yWindow="675" windowWidth="21218" windowHeight="12593" xr2:uid="{663B75C4-4EF0-43BA-B2A2-705907C78B86}"/>
   </bookViews>
   <sheets>
     <sheet name="FRED Graph" sheetId="1" r:id="rId1"/>
@@ -426,7 +426,7 @@
   <dimension ref="A1:B108"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A87" workbookViewId="0">
-      <selection activeCell="B109" sqref="B109"/>
+      <selection activeCell="A109" sqref="A109:XFD109"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.6640625" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
@@ -1252,10 +1252,10 @@
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A108" s="1">
-        <v>45777</v>
+        <v>45779</v>
       </c>
       <c r="B108" s="2">
-        <v>1.94</v>
+        <v>2.06</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Change project structure, move read/write operations to functions, combine projections into one parquet file
</commit_message>
<xml_diff>
--- a/input_output/input_dir/DFII10.xlsx
+++ b/input_output/input_dir/DFII10.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Mac\Home\Python_Projects\sp500_earn_price\input_output\input_dir\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54B2388B-4F60-43A2-BD65-EDE3CCC837B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6381A2DC-9917-43CF-80AD-95A7D20C5A06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="675" yWindow="675" windowWidth="21218" windowHeight="12593" xr2:uid="{663B75C4-4EF0-43BA-B2A2-705907C78B86}"/>
+    <workbookView xWindow="1470" yWindow="1087" windowWidth="21217" windowHeight="12593" xr2:uid="{663B75C4-4EF0-43BA-B2A2-705907C78B86}"/>
   </bookViews>
   <sheets>
     <sheet name="FRED Graph" sheetId="1" r:id="rId1"/>
@@ -423,10 +423,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23184F55-AF2F-421E-BC51-13A1C6FC6898}">
-  <dimension ref="A1:B108"/>
+  <dimension ref="A1:B115"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A87" workbookViewId="0">
-      <selection activeCell="A109" sqref="A109:XFD109"/>
+      <selection activeCell="B116" sqref="B116"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.6640625" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
@@ -1258,6 +1258,62 @@
         <v>2.06</v>
       </c>
     </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A109" s="1">
+        <v>45786</v>
+      </c>
+      <c r="B109" s="2">
+        <v>2.08</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A110" s="1">
+        <v>45803</v>
+      </c>
+      <c r="B110" s="2">
+        <v>2.11</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A111" s="1">
+        <v>45807</v>
+      </c>
+      <c r="B111" s="2">
+        <v>2.11</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A112" s="1">
+        <v>45811</v>
+      </c>
+      <c r="B112" s="2">
+        <v>2.14</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A113" s="1">
+        <v>45820</v>
+      </c>
+      <c r="B113" s="2">
+        <v>2.11</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A114" s="1">
+        <v>45825</v>
+      </c>
+      <c r="B114" s="2">
+        <v>2.08</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A115" s="1">
+        <v>45838</v>
+      </c>
+      <c r="B115" s="2">
+        <v>1.95</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
tidy code, treat bug
</commit_message>
<xml_diff>
--- a/input_output/input_dir/DFII10.xlsx
+++ b/input_output/input_dir/DFII10.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Mac\Home\Python_Projects\sp500_earn_price\input_output\input_dir\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6381A2DC-9917-43CF-80AD-95A7D20C5A06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A92B0433-D756-4D83-BE95-660AFA534CB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1470" yWindow="1087" windowWidth="21217" windowHeight="12593" xr2:uid="{663B75C4-4EF0-43BA-B2A2-705907C78B86}"/>
   </bookViews>
@@ -423,10 +423,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23184F55-AF2F-421E-BC51-13A1C6FC6898}">
-  <dimension ref="A1:B115"/>
+  <dimension ref="A1:B116"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A87" workbookViewId="0">
-      <selection activeCell="B116" sqref="B116"/>
+      <selection activeCell="B117" sqref="B117"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.6640625" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
@@ -1314,6 +1314,14 @@
         <v>1.95</v>
       </c>
     </row>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A116" s="1">
+        <v>45845</v>
+      </c>
+      <c r="B116" s="2">
+        <v>2.0499999999999998</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
add recent input and run main branch
</commit_message>
<xml_diff>
--- a/input_output/input_dir/DFII10.xlsx
+++ b/input_output/input_dir/DFII10.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Mac\Home\Python_Projects\sp500_earn_price\input_output\input_dir\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A92B0433-D756-4D83-BE95-660AFA534CB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCD91828-5E6F-4BF3-8114-2B7347311578}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1470" yWindow="1087" windowWidth="21217" windowHeight="12593" xr2:uid="{663B75C4-4EF0-43BA-B2A2-705907C78B86}"/>
+    <workbookView xWindow="368" yWindow="368" windowWidth="21217" windowHeight="12592" xr2:uid="{663B75C4-4EF0-43BA-B2A2-705907C78B86}"/>
   </bookViews>
   <sheets>
     <sheet name="FRED Graph" sheetId="1" r:id="rId1"/>
@@ -423,10 +423,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23184F55-AF2F-421E-BC51-13A1C6FC6898}">
-  <dimension ref="A1:B116"/>
+  <dimension ref="A1:B117"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A87" workbookViewId="0">
-      <selection activeCell="B117" sqref="B117"/>
+      <selection activeCell="A118" sqref="A118"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.6640625" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
@@ -1322,6 +1322,14 @@
         <v>2.0499999999999998</v>
       </c>
     </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A117" s="1">
+        <v>45849</v>
+      </c>
+      <c r="B117" s="2">
+        <v>2.06</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>